<commit_message>
Including date_variable and date_forma parameters, to fix issue with date variable
</commit_message>
<xml_diff>
--- a/inputs/dataset_1.xlsx
+++ b/inputs/dataset_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7110"/>
+    <workbookView windowWidth="27975" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>data_tidy</t>
+    <t>DATE_VARIABLE</t>
   </si>
   <si>
     <t>fs_pim</t>
@@ -67,11 +67,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="181" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -106,16 +106,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -129,8 +137,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,6 +147,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,18 +182,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -182,7 +198,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -197,32 +213,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -231,6 +224,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -249,7 +249,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -261,7 +297,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,19 +357,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,37 +393,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,79 +417,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,17 +452,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,17 +502,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -516,165 +534,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -692,7 +692,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1016,26 +1016,26 @@
   <dimension ref="A1:O253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O1" sqref="A1:O1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10.7533333333333" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.37333333333333" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.37333333333333" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.37333333333333" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.3733333333333" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.37333333333333" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.6266666666667" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.6266666666667" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.8733333333333" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.875" style="4" customWidth="1"/>
     <col min="10" max="10" width="16.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="12.6266666666667" style="4" customWidth="1"/>
-    <col min="12" max="12" width="14.8733333333333" style="4" customWidth="1"/>
-    <col min="13" max="13" width="18.8733333333333" style="4" customWidth="1"/>
-    <col min="14" max="14" width="20.6266666666667" style="4" customWidth="1"/>
-    <col min="15" max="15" width="12.8733333333333" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12.625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="14.875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="18.875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="20.625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="4" customWidth="1"/>
     <col min="16" max="16378" width="9" style="2"/>
   </cols>
   <sheetData>

</xml_diff>